<commit_message>
2019 12 19 corrigido o processo de consulta
</commit_message>
<xml_diff>
--- a/testemunhoweb/logs/janeiroOficial.xlsx
+++ b/testemunhoweb/logs/janeiroOficial.xlsx
@@ -566,13 +566,13 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="18.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.05"/>
@@ -581,14 +581,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.03"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="12" style="1" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="1023" style="2" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="n">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1414,10 +1414,10 @@
   <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="A1:K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.3"/>
   </cols>

</xml_diff>